<commit_message>
updated south korea files
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_RevisionComplete\bldgs\BCEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_Complete\bldgs\BCEU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322473FB-2C37-40DC-935D-798D4FE7EFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1527DC64-7A96-4D5E-87C3-C62693DBEAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="340" windowWidth="24420" windowHeight="20560" tabRatio="952" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7230" yWindow="850" windowWidth="28800" windowHeight="15460" tabRatio="952" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SYCEU" sheetId="35" r:id="rId2"/>
     <sheet name="Forecast" sheetId="39" r:id="rId3"/>
-    <sheet name="Snopshot2040" sheetId="40" r:id="rId4"/>
+    <sheet name="Snapshot2040" sheetId="40" r:id="rId4"/>
     <sheet name="Commercial_calculation" sheetId="36" r:id="rId5"/>
     <sheet name="Urban_res_calculation" sheetId="37" r:id="rId6"/>
     <sheet name="Rural_res_calculation" sheetId="38" r:id="rId7"/>
@@ -175,10 +175,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>1 TOE to mBTU</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>1kWh to BTU</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -285,6 +281,10 @@
   </si>
   <si>
     <t>* this tab is for validating the outcome by cross checking</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 TOE to mmBTU</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="13" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B30" s="13">
         <v>39.683100000000003</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="16">
         <v>3412.1419999999998</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="13">
         <v>43.54</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="13">
         <v>947.81700000000001</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="17">
         <v>4600</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="18">
         <v>3.968318</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="13">
         <v>50.4</v>
@@ -1286,13 +1286,13 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="19">
         <v>0.91800000000000004</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
@@ -1433,7 +1433,7 @@
   </sheetPr>
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -16026,25 +16026,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -16282,25 +16282,25 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -16535,25 +16535,25 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="D25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="E25" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="F25" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -22305,7 +22305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CFF0D5-CCA6-41D0-9ADB-4D3C10D15974}">
   <dimension ref="A2:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -22317,10 +22317,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -22405,15 +22405,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="4">
         <v>-1.1000000000000001E-2</v>
@@ -22421,7 +22421,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="4">
         <v>1.2E-2</v>
@@ -22429,7 +22429,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -22437,7 +22437,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="4">
         <v>4.0000000000000001E-3</v>
@@ -22445,7 +22445,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="4">
         <v>1.6E-2</v>
@@ -22453,7 +22453,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="4">
         <v>1E-3</v>
@@ -22461,10 +22461,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -22483,7 +22483,7 @@
         <v>-8.6999999999999994E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -22560,7 +22560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369EACEB-8E8C-4A24-B652-74E6055FDD6D}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
@@ -22577,31 +22577,31 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="I1" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -22997,31 +22997,31 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="D14" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="E14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="F14" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="G14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="I14" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="J14" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
@@ -23416,31 +23416,31 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="20" t="s">
-        <v>45</v>
-      </c>
       <c r="I27" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -23877,7 +23877,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -23903,12 +23903,12 @@
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
@@ -25339,7 +25339,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
@@ -26770,7 +26770,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
         <v>2019</v>
@@ -28201,7 +28201,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
         <v>2019</v>
@@ -29632,7 +29632,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
         <v>2019</v>
@@ -31063,7 +31063,7 @@
     </row>
     <row r="63" spans="1:33" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1">
         <v>2019</v>
@@ -32516,12 +32516,12 @@
   <sheetData>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
@@ -33952,7 +33952,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
@@ -35383,7 +35383,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
         <v>2019</v>
@@ -36814,7 +36814,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
         <v>2019</v>
@@ -38245,7 +38245,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
         <v>2019</v>
@@ -39676,7 +39676,7 @@
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1">
         <v>2019</v>
@@ -41129,12 +41129,12 @@
   <sheetData>
     <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A2" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
@@ -42587,7 +42587,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>2019</v>
@@ -44040,7 +44040,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1">
         <v>2019</v>
@@ -45493,7 +45493,7 @@
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1">
         <v>2019</v>
@@ -46946,7 +46946,7 @@
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
         <v>2019</v>
@@ -48399,7 +48399,7 @@
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A63" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B63" s="1">
         <v>2019</v>

</xml_diff>